<commit_message>
treeview dispensa eletronica api pncp
</commit_message>
<xml_diff>
--- a/controle_dispensa_eletronica.xlsx
+++ b/controle_dispensa_eletronica.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="265">
   <si>
     <t>ID Processo</t>
   </si>
@@ -154,345 +154,327 @@
     <t>codigoMunicipioIbge</t>
   </si>
   <si>
-    <t>DE 90001/2024</t>
-  </si>
-  <si>
-    <t>DE 90002/2024</t>
-  </si>
-  <si>
     <t>DE 90003/2024</t>
   </si>
   <si>
-    <t>DE 90004/2024</t>
-  </si>
-  <si>
     <t>DE 90005/2024</t>
   </si>
   <si>
-    <t>DE 90006/2024</t>
-  </si>
-  <si>
-    <t>DE 90007/2024</t>
-  </si>
-  <si>
-    <t>DE 90008/2024</t>
-  </si>
-  <si>
-    <t>DE 90009/2024</t>
-  </si>
-  <si>
-    <t>DE 90010/2024</t>
-  </si>
-  <si>
-    <t>DE 90011/2024</t>
-  </si>
-  <si>
-    <t>DE 90012/2024</t>
-  </si>
-  <si>
-    <t>DE 90013/2024</t>
-  </si>
-  <si>
-    <t>DE 90014/2024</t>
-  </si>
-  <si>
-    <t>DE 90015/2024</t>
-  </si>
-  <si>
-    <t>DE 90016/2024</t>
-  </si>
-  <si>
-    <t>DE 90017/2024</t>
+    <t>DE 06/2024</t>
+  </si>
+  <si>
+    <t>DE 07/2024</t>
+  </si>
+  <si>
+    <t>DE 08/2024</t>
+  </si>
+  <si>
+    <t>DE 09/2024</t>
+  </si>
+  <si>
+    <t>DE 10/2024</t>
+  </si>
+  <si>
+    <t>DE 11/2024</t>
+  </si>
+  <si>
+    <t>DE 12/2024</t>
+  </si>
+  <si>
+    <t>DE 13/2024</t>
+  </si>
+  <si>
+    <t>DE 14/2024</t>
+  </si>
+  <si>
+    <t>DE 15/2024</t>
+  </si>
+  <si>
+    <t>DE 16/2024</t>
+  </si>
+  <si>
+    <t>DE 17/2024</t>
+  </si>
+  <si>
+    <t>DE 18/2024</t>
+  </si>
+  <si>
+    <t>DE 19/2024</t>
+  </si>
+  <si>
+    <t>DE 20/2024</t>
+  </si>
+  <si>
+    <t>DE 21/2024</t>
+  </si>
+  <si>
+    <t>DE 22/2024</t>
+  </si>
+  <si>
+    <t>DE 23/2024</t>
+  </si>
+  <si>
+    <t>DE 26/2024</t>
+  </si>
+  <si>
+    <t>DE 27/2024</t>
+  </si>
+  <si>
+    <t>DE 28/2024</t>
+  </si>
+  <si>
+    <t>DE 29/2024</t>
+  </si>
+  <si>
+    <t>DE 30/2024</t>
+  </si>
+  <si>
+    <t>DE 31/2024</t>
+  </si>
+  <si>
+    <t>DE 32/2024</t>
+  </si>
+  <si>
+    <t>DE 33/2024</t>
+  </si>
+  <si>
+    <t>DE 34/2024</t>
+  </si>
+  <si>
+    <t>DE 35/2024</t>
+  </si>
+  <si>
+    <t>DE 40/2024</t>
+  </si>
+  <si>
+    <t>DE 37/2024</t>
+  </si>
+  <si>
+    <t>DE 38/2024</t>
+  </si>
+  <si>
+    <t>DE 39/2024</t>
+  </si>
+  <si>
+    <t>DE 41/2024</t>
+  </si>
+  <si>
+    <t>DE 42/2024</t>
+  </si>
+  <si>
+    <t>DE 43/2024</t>
+  </si>
+  <si>
+    <t>DE 44/2024</t>
+  </si>
+  <si>
+    <t>DE 45/2024</t>
+  </si>
+  <si>
+    <t>DE 46/2024</t>
+  </si>
+  <si>
+    <t>DE 47/2024</t>
+  </si>
+  <si>
+    <t>DE 48/2024</t>
+  </si>
+  <si>
+    <t>DE 90038/2024</t>
   </si>
   <si>
     <t>DE 90018/2024</t>
   </si>
   <si>
-    <t>DE 90019/2024</t>
-  </si>
-  <si>
-    <t>DE 90020/2024</t>
-  </si>
-  <si>
-    <t>DE 90021/2024</t>
-  </si>
-  <si>
-    <t>DE 90022/2024</t>
-  </si>
-  <si>
-    <t>DE 90023/2024</t>
-  </si>
-  <si>
-    <t>DE 90024/2024</t>
-  </si>
-  <si>
-    <t>DE 90025/2024</t>
-  </si>
-  <si>
-    <t>DE 90026/2024</t>
-  </si>
-  <si>
-    <t>DE 90027/2024</t>
-  </si>
-  <si>
-    <t>DE 90028/2024</t>
-  </si>
-  <si>
-    <t>DE 90029/2024</t>
-  </si>
-  <si>
-    <t>DE 90030/2024</t>
-  </si>
-  <si>
-    <t>DE 90031/2024</t>
-  </si>
-  <si>
-    <t>DE 90032/2024</t>
-  </si>
-  <si>
-    <t>DE 90033/2024</t>
-  </si>
-  <si>
-    <t>DE 90034/2024</t>
-  </si>
-  <si>
-    <t>DE 90035/2024</t>
-  </si>
-  <si>
-    <t>DE 90036/2024</t>
-  </si>
-  <si>
-    <t>DE 90037/2024</t>
-  </si>
-  <si>
-    <t>DE 90038/2024</t>
-  </si>
-  <si>
-    <t>DE 90039/2024</t>
-  </si>
-  <si>
-    <t>DE 90040/2024</t>
-  </si>
-  <si>
-    <t>DE 90041/2024</t>
-  </si>
-  <si>
-    <t>DE 90042/2024</t>
-  </si>
-  <si>
-    <t>DE 90043/2024</t>
-  </si>
-  <si>
-    <t>DE 90044/2024</t>
-  </si>
-  <si>
-    <t>DE 90045/2024</t>
-  </si>
-  <si>
-    <t>DE 90046/2024</t>
-  </si>
-  <si>
-    <t>DE 90047/2024</t>
-  </si>
-  <si>
-    <t>DE 90048/2024</t>
+    <t>DE 90100/2024</t>
   </si>
   <si>
     <t>Dispensa Eletrônica</t>
   </si>
   <si>
-    <t>90001</t>
-  </si>
-  <si>
-    <t>90002</t>
-  </si>
-  <si>
     <t>90003</t>
   </si>
   <si>
-    <t>90004</t>
-  </si>
-  <si>
     <t>90005</t>
   </si>
   <si>
-    <t>90006</t>
-  </si>
-  <si>
-    <t>90007</t>
-  </si>
-  <si>
-    <t>90008</t>
-  </si>
-  <si>
-    <t>90009</t>
-  </si>
-  <si>
-    <t>90010</t>
-  </si>
-  <si>
-    <t>90011</t>
-  </si>
-  <si>
-    <t>90012</t>
-  </si>
-  <si>
-    <t>90013</t>
-  </si>
-  <si>
-    <t>90014</t>
-  </si>
-  <si>
-    <t>90015</t>
-  </si>
-  <si>
-    <t>90016</t>
-  </si>
-  <si>
-    <t>90017</t>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>90038</t>
   </si>
   <si>
     <t>90018</t>
   </si>
   <si>
-    <t>90019</t>
-  </si>
-  <si>
-    <t>90020</t>
-  </si>
-  <si>
-    <t>90021</t>
-  </si>
-  <si>
-    <t>90022</t>
-  </si>
-  <si>
-    <t>90023</t>
-  </si>
-  <si>
-    <t>90024</t>
-  </si>
-  <si>
-    <t>90025</t>
-  </si>
-  <si>
-    <t>90026</t>
-  </si>
-  <si>
-    <t>90027</t>
-  </si>
-  <si>
-    <t>90028</t>
-  </si>
-  <si>
-    <t>90029</t>
-  </si>
-  <si>
-    <t>90030</t>
-  </si>
-  <si>
-    <t>90031</t>
-  </si>
-  <si>
-    <t>90032</t>
-  </si>
-  <si>
-    <t>90033</t>
-  </si>
-  <si>
-    <t>90034</t>
-  </si>
-  <si>
-    <t>90035</t>
-  </si>
-  <si>
-    <t>90036</t>
-  </si>
-  <si>
-    <t>90037</t>
-  </si>
-  <si>
-    <t>90038</t>
-  </si>
-  <si>
-    <t>90039</t>
-  </si>
-  <si>
-    <t>90040</t>
-  </si>
-  <si>
-    <t>90041</t>
-  </si>
-  <si>
-    <t>90042</t>
-  </si>
-  <si>
-    <t>90043</t>
-  </si>
-  <si>
-    <t>90044</t>
-  </si>
-  <si>
-    <t>90045</t>
-  </si>
-  <si>
-    <t>90046</t>
-  </si>
-  <si>
-    <t>90047</t>
-  </si>
-  <si>
-    <t>90048</t>
+    <t>90100</t>
   </si>
   <si>
     <t>2024</t>
   </si>
   <si>
+    <t>Planejamento</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
     <t>Homologado</t>
   </si>
   <si>
-    <t>Arquivado</t>
-  </si>
-  <si>
-    <t>Planejamento</t>
-  </si>
-  <si>
-    <t>Aprovado</t>
-  </si>
-  <si>
-    <t>62055.000565/2024-94</t>
+    <t>Sessão Pública</t>
+  </si>
+  <si>
+    <t>Empenhado</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>62055.001118/2024-52</t>
+  </si>
+  <si>
+    <t>62055.001071/2024-27</t>
+  </si>
+  <si>
+    <t>62055.001072/2024-71</t>
+  </si>
+  <si>
+    <t>62055.001314/2024-27</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>62055.001855/2024-55</t>
+  </si>
+  <si>
+    <t>62055.001829/2024-27</t>
+  </si>
+  <si>
+    <t>62055.001951/2024-01</t>
   </si>
   <si>
     <t>62055.000957/2024-53</t>
   </si>
   <si>
-    <t>62055.001118/2024-52</t>
-  </si>
-  <si>
-    <t>62055.001070/2024-82</t>
-  </si>
-  <si>
-    <t>62055.001071/2024-27</t>
-  </si>
-  <si>
-    <t>62055.001072/2024-71</t>
-  </si>
-  <si>
-    <t>62055.001314/2024-27</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>62055.001855/2024-55</t>
-  </si>
-  <si>
-    <t>62055.001829/2024-27</t>
-  </si>
-  <si>
-    <t>62055.001951/2024-01</t>
-  </si>
-  <si>
     <t>63402.000196/2024-13</t>
   </si>
   <si>
@@ -511,12 +493,6 @@
     <t>63402.000513/2024-93</t>
   </si>
   <si>
-    <t>63402.000548/2024-22</t>
-  </si>
-  <si>
-    <t>63402.000538/2024-97</t>
-  </si>
-  <si>
     <t>63402.000539/2024-31</t>
   </si>
   <si>
@@ -538,7 +514,7 @@
     <t>63402.001006/2024-77</t>
   </si>
   <si>
-    <t>63402.001129/2024-16</t>
+    <t>62055.5555/2024-50</t>
   </si>
   <si>
     <t>63402.001294/2024-60</t>
@@ -547,7 +523,7 @@
     <t>63402.001499/2024-45</t>
   </si>
   <si>
-    <t>63402.001492/2024-23</t>
+    <t>63402.001644/2024-98</t>
   </si>
   <si>
     <t>63402.001519/2024-88</t>
@@ -559,9 +535,6 @@
     <t>63402.001637/2024-96</t>
   </si>
   <si>
-    <t>63402.001644/2024-98</t>
-  </si>
-  <si>
     <t>63402.001650/2024-45</t>
   </si>
   <si>
@@ -571,19 +544,13 @@
     <t>63402.001689/2024-62</t>
   </si>
   <si>
-    <t>63402.001690/2024-97</t>
-  </si>
-  <si>
-    <t>63402.001718/2024-96</t>
-  </si>
-  <si>
-    <t>63402.001719/2024-31</t>
-  </si>
-  <si>
-    <t>63402.001720/2024-65</t>
-  </si>
-  <si>
-    <t>63402.001797/2024-35</t>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>62055.00000/2024-44</t>
   </si>
   <si>
     <t>Material</t>
@@ -592,18 +559,9 @@
     <t>Serviço</t>
   </si>
   <si>
-    <t>Copos Descartáveis</t>
-  </si>
-  <si>
-    <t>Legumes</t>
-  </si>
-  <si>
     <t>Instalação de Ar Condicionado</t>
   </si>
   <si>
-    <t>Brasão Institucional</t>
-  </si>
-  <si>
     <t>Material de Comunicação Social</t>
   </si>
   <si>
@@ -619,7 +577,7 @@
     <t>Display de acrílico A4</t>
   </si>
   <si>
-    <t>Ar-Condicionado e Fragmentadora</t>
+    <t>Ar-Condicionado e Fragmentadora de Papel</t>
   </si>
   <si>
     <t>Tampo de Vidro</t>
@@ -628,7 +586,7 @@
     <t>Painel de Anúncio Backdrop</t>
   </si>
   <si>
-    <t>Medalhas para Regata</t>
+    <t xml:space="preserve"> Materiais de Divulgação das Regatas do Circuito Poder Marítimo</t>
   </si>
   <si>
     <t>Scanner Automotivo</t>
@@ -637,67 +595,52 @@
     <t>Moedas Institucionais</t>
   </si>
   <si>
-    <t>Batata, Cenoura, Abóbora e Banana</t>
+    <t xml:space="preserve"> Gêneros Alimentícios (hortifrúti)</t>
   </si>
   <si>
     <t>Bolo Confeitado</t>
   </si>
   <si>
-    <t>Dedetização e Desratização</t>
-  </si>
-  <si>
-    <t>Limpeza de Coifas</t>
-  </si>
-  <si>
-    <t>Materiais de Limpeza</t>
-  </si>
-  <si>
-    <t>Materiais de Expediente</t>
-  </si>
-  <si>
-    <t>Câmera fotográfica Digital e Acessórios</t>
+    <t xml:space="preserve"> Dedetização e Desratização</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Limpeza, Higienização e Remoção de Gordura de Coifas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> materiais de Limpeza</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Materiais de Expediente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Câmera fotográfica Digital e Acessórios</t>
   </si>
   <si>
     <t>Material de Representação</t>
   </si>
   <si>
-    <t>Publicidade Legal</t>
-  </si>
-  <si>
-    <t>Detergente, Cera, entre outros.</t>
-  </si>
-  <si>
-    <t>Abóbora, Batata e Abobrinha</t>
-  </si>
-  <si>
-    <t>Acelga, Alface e Couve</t>
-  </si>
-  <si>
-    <t>Maçã, Pera e Tangerina</t>
-  </si>
-  <si>
-    <t>Mandioca, Vagem e Brócolis</t>
-  </si>
-  <si>
-    <t>Aparelho Telefônico</t>
+    <t>Gêneros Alimentícios (hortifrúti)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Material de Comunicação Social</t>
   </si>
   <si>
     <t>Notebooks</t>
   </si>
   <si>
-    <t>Cadeiras de Escritório</t>
-  </si>
-  <si>
-    <t>Material de Copa e Cozinha</t>
-  </si>
-  <si>
-    <t>Rodas dos Contêineres do Rancho</t>
-  </si>
-  <si>
-    <t>Armário de CAV</t>
-  </si>
-  <si>
-    <t>Caixas Hotbox</t>
+    <t xml:space="preserve"> Cadeiras de Escritório</t>
+  </si>
+  <si>
+    <t>Material de Copa e Cozinha e Rancho</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>teste2</t>
+  </si>
+  <si>
+    <t>Material de Limpeza</t>
   </si>
   <si>
     <t>Instalação de Piso Vinílico</t>
@@ -706,10 +649,7 @@
     <t>Água Mineral</t>
   </si>
   <si>
-    <t>Papel A4</t>
-  </si>
-  <si>
-    <t>Detergente e Saco de Lixo 100L</t>
+    <t>Material de Expediente</t>
   </si>
   <si>
     <t>Mesa</t>
@@ -721,19 +661,60 @@
     <t>Confecção de painel</t>
   </si>
   <si>
-    <t>Capacho</t>
-  </si>
-  <si>
-    <t>Requeijão, Presunto e Mortadela</t>
-  </si>
-  <si>
-    <t>Queijo e Manteiga</t>
-  </si>
-  <si>
-    <t>Ovos de Galinha e Codorna</t>
-  </si>
-  <si>
-    <t>Bebedouro</t>
+    <t>capacho</t>
+  </si>
+  <si>
+    <t>Gêneros alimentícios (Laticínios)</t>
+  </si>
+  <si>
+    <t>Gêneros Alimentícios (Laticínios)</t>
+  </si>
+  <si>
+    <t>Microfone</t>
+  </si>
+  <si>
+    <t>testex</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>4 (quatro) meses</t>
+  </si>
+  <si>
+    <t>3 (três) meses</t>
+  </si>
+  <si>
+    <t>2024-09-12</t>
+  </si>
+  <si>
+    <t>2024-09-13</t>
+  </si>
+  <si>
+    <t>2024-09-21</t>
+  </si>
+  <si>
+    <t>2024-09-20</t>
+  </si>
+  <si>
+    <t>2024-09-11</t>
+  </si>
+  <si>
+    <t>2024-06-04</t>
+  </si>
+  <si>
+    <t>OLIVEIRA
+Capitão de Corveta (IM)
+Operador de Dispensa Eletrônica</t>
+  </si>
+  <si>
+    <t>Menor Preço</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
   </si>
   <si>
     <t>787000</t>
@@ -742,37 +723,102 @@
     <t>787010</t>
   </si>
   <si>
+    <t>787700</t>
+  </si>
+  <si>
     <t>COMANDO DO 7º DISTRITO NAVAL</t>
   </si>
   <si>
     <t>CENTRO DE INTENDÊNCIA DA MARINHA EM BRASÍLIA</t>
   </si>
   <si>
+    <t>HOSPITAL NAVAL DE BRASÍLIA</t>
+  </si>
+  <si>
     <t>Com7ºDN</t>
   </si>
   <si>
     <t>CeIMBra</t>
   </si>
   <si>
+    <t>HNBRA</t>
+  </si>
+  <si>
+    <t>Divisão de Abastecimento</t>
+  </si>
+  <si>
     <t>Divisão de Municiamento</t>
   </si>
   <si>
+    <t>Administração</t>
+  </si>
+  <si>
     <t>Divisão de Administração</t>
   </si>
   <si>
-    <t>Pagamento</t>
-  </si>
-  <si>
-    <t>Administração CeIMBra-50</t>
-  </si>
-  <si>
-    <t>Administração</t>
+    <t>Municiamento</t>
   </si>
   <si>
     <t>Secretaria do Diretor</t>
   </si>
   <si>
-    <t>Divisão de Subsistência</t>
+    <t>CeIMNi</t>
+  </si>
+  <si>
+    <t>RAMON DE LIMA FERNANDES
+Capitão de Corveta (IM)
+Encarregado da Divisão de Subsistência</t>
+  </si>
+  <si>
+    <t>BRUNO SANTA RITA MOREIRA
+Capitão de Fragata (IM)
+Ordenador de Despesa</t>
+  </si>
+  <si>
+    <t>THIAGO MARTINS AMORIM
+Capitão de Fragata (IM)
+Agente Fiscal</t>
+  </si>
+  <si>
+    <t>RANA
+Capitão-Tenente (IM)
+Gerente de Crédito</t>
+  </si>
+  <si>
+    <t>Necessário</t>
+  </si>
+  <si>
+    <t>testes</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>estse</t>
+  </si>
+  <si>
+    <t>tes</t>
+  </si>
+  <si>
+    <t>R$ 500,00</t>
+  </si>
+  <si>
+    <t>002900</t>
+  </si>
+  <si>
+    <t>010949</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>5300108</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1176,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT49"/>
+  <dimension ref="A1:AT46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1281,34 +1327,121 @@
         <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" t="s">
         <v>144</v>
       </c>
-      <c r="F2" t="s">
-        <v>148</v>
-      </c>
       <c r="G2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H2" t="s">
-        <v>192</v>
+        <v>181</v>
+      </c>
+      <c r="I2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K2" t="s">
+        <v>229</v>
+      </c>
+      <c r="L2" t="s">
+        <v>230</v>
+      </c>
+      <c r="M2" t="s">
+        <v>231</v>
+      </c>
+      <c r="N2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O2" t="s">
+        <v>223</v>
       </c>
       <c r="P2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q2" t="s">
+        <v>236</v>
+      </c>
+      <c r="R2" t="s">
+        <v>239</v>
+      </c>
+      <c r="S2" t="s">
         <v>242</v>
       </c>
-      <c r="R2" t="s">
-        <v>244</v>
+      <c r="T2" t="s">
+        <v>249</v>
+      </c>
+      <c r="U2" t="s">
+        <v>250</v>
+      </c>
+      <c r="V2" t="s">
+        <v>251</v>
+      </c>
+      <c r="W2" t="s">
+        <v>252</v>
+      </c>
+      <c r="X2" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:46">
@@ -1316,34 +1449,34 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G3" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="P3" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="R3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:46">
@@ -1351,34 +1484,121 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
         <v>94</v>
       </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H4" t="s">
-        <v>194</v>
+        <v>183</v>
+      </c>
+      <c r="I4" t="s">
+        <v>220</v>
+      </c>
+      <c r="J4" t="s">
+        <v>224</v>
+      </c>
+      <c r="K4" t="s">
+        <v>229</v>
+      </c>
+      <c r="L4" t="s">
+        <v>230</v>
+      </c>
+      <c r="M4" t="s">
+        <v>231</v>
+      </c>
+      <c r="N4" t="s">
+        <v>232</v>
+      </c>
+      <c r="O4" t="s">
+        <v>224</v>
       </c>
       <c r="P4" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="R4" t="s">
-        <v>244</v>
+        <v>239</v>
+      </c>
+      <c r="S4" t="s">
+        <v>220</v>
+      </c>
+      <c r="T4" t="s">
+        <v>249</v>
+      </c>
+      <c r="U4" t="s">
+        <v>250</v>
+      </c>
+      <c r="V4" t="s">
+        <v>251</v>
+      </c>
+      <c r="W4" t="s">
+        <v>252</v>
+      </c>
+      <c r="X4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:46">
@@ -1386,34 +1606,121 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G5" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H5" t="s">
-        <v>195</v>
+        <v>184</v>
+      </c>
+      <c r="I5" t="s">
+        <v>220</v>
+      </c>
+      <c r="J5" t="s">
+        <v>224</v>
+      </c>
+      <c r="K5" t="s">
+        <v>229</v>
+      </c>
+      <c r="L5" t="s">
+        <v>230</v>
+      </c>
+      <c r="M5" t="s">
+        <v>231</v>
+      </c>
+      <c r="N5" t="s">
+        <v>232</v>
+      </c>
+      <c r="O5" t="s">
+        <v>224</v>
       </c>
       <c r="P5" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="R5" t="s">
-        <v>244</v>
+        <v>239</v>
+      </c>
+      <c r="S5" t="s">
+        <v>220</v>
+      </c>
+      <c r="T5" t="s">
+        <v>249</v>
+      </c>
+      <c r="U5" t="s">
+        <v>250</v>
+      </c>
+      <c r="V5" t="s">
+        <v>251</v>
+      </c>
+      <c r="W5" t="s">
+        <v>252</v>
+      </c>
+      <c r="X5" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:46">
@@ -1421,34 +1728,31 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G6" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="H6" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="P6" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>237</v>
+      </c>
+      <c r="R6" t="s">
         <v>240</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>242</v>
-      </c>
-      <c r="R6" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:46">
@@ -1456,34 +1760,34 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G7" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H7" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="P7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="Q7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="R7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:46">
@@ -1491,34 +1795,34 @@
         <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G8" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H8" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="P8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="R8" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:46">
@@ -1526,31 +1830,31 @@
         <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F9" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H9" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="P9" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q9" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R9" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:46">
@@ -1558,34 +1862,31 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F10" t="s">
-        <v>156</v>
-      </c>
-      <c r="G10" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="H10" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="P10" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>237</v>
+      </c>
+      <c r="R10" t="s">
         <v>240</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>242</v>
-      </c>
-      <c r="R10" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:46">
@@ -1593,34 +1894,31 @@
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E11" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F11" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" t="s">
         <v>190</v>
       </c>
-      <c r="H11" t="s">
-        <v>201</v>
-      </c>
       <c r="P11" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q11" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="R11" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:46">
@@ -1628,31 +1926,130 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F12" t="s">
-        <v>155</v>
+        <v>148</v>
+      </c>
+      <c r="G12" t="s">
+        <v>179</v>
       </c>
       <c r="H12" t="s">
-        <v>202</v>
+        <v>191</v>
+      </c>
+      <c r="I12" t="s">
+        <v>220</v>
+      </c>
+      <c r="J12" t="s">
+        <v>225</v>
+      </c>
+      <c r="K12" t="s">
+        <v>229</v>
+      </c>
+      <c r="L12" t="s">
+        <v>230</v>
+      </c>
+      <c r="M12" t="s">
+        <v>231</v>
+      </c>
+      <c r="N12" t="s">
+        <v>232</v>
+      </c>
+      <c r="O12" t="s">
+        <v>225</v>
       </c>
       <c r="P12" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="Q12" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="R12" t="s">
-        <v>245</v>
+        <v>239</v>
+      </c>
+      <c r="S12" t="s">
+        <v>220</v>
+      </c>
+      <c r="T12" t="s">
+        <v>249</v>
+      </c>
+      <c r="U12" t="s">
+        <v>250</v>
+      </c>
+      <c r="V12" t="s">
+        <v>251</v>
+      </c>
+      <c r="W12" t="s">
+        <v>252</v>
+      </c>
+      <c r="X12" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>260</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>220</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>263</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:46">
@@ -1660,31 +2057,31 @@
         <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H13" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="P13" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q13" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R13" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:46">
@@ -1692,34 +2089,31 @@
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F14" t="s">
-        <v>158</v>
-      </c>
-      <c r="G14" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="H14" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="P14" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q14" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="R14" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:46">
@@ -1727,31 +2121,124 @@
         <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E15" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F15" t="s">
-        <v>155</v>
+        <v>148</v>
+      </c>
+      <c r="G15" t="s">
+        <v>179</v>
       </c>
       <c r="H15" t="s">
-        <v>205</v>
+        <v>194</v>
+      </c>
+      <c r="I15" t="s">
+        <v>220</v>
+      </c>
+      <c r="J15" t="s">
+        <v>225</v>
+      </c>
+      <c r="K15" t="s">
+        <v>229</v>
+      </c>
+      <c r="L15" t="s">
+        <v>230</v>
+      </c>
+      <c r="M15" t="s">
+        <v>231</v>
+      </c>
+      <c r="N15" t="s">
+        <v>232</v>
+      </c>
+      <c r="O15" t="s">
+        <v>225</v>
       </c>
       <c r="P15" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q15" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R15" t="s">
-        <v>245</v>
+        <v>240</v>
+      </c>
+      <c r="S15" t="s">
+        <v>220</v>
+      </c>
+      <c r="T15" t="s">
+        <v>249</v>
+      </c>
+      <c r="U15" t="s">
+        <v>250</v>
+      </c>
+      <c r="V15" t="s">
+        <v>251</v>
+      </c>
+      <c r="W15" t="s">
+        <v>252</v>
+      </c>
+      <c r="X15" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>260</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:46">
@@ -1759,1225 +2246,1447 @@
         <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H16" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="P16" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q16" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D17" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F17" t="s">
-        <v>149</v>
-      </c>
-      <c r="G17" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="H17" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="P17" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>237</v>
+      </c>
+      <c r="R17" t="s">
         <v>240</v>
       </c>
-      <c r="Q17" t="s">
-        <v>242</v>
-      </c>
-      <c r="R17" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F18" t="s">
         <v>155</v>
       </c>
       <c r="H18" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="P18" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q18" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R18" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E19" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F19" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="H19" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="P19" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q19" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R19" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E20" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F20" t="s">
-        <v>160</v>
-      </c>
-      <c r="G20" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="H20" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="P20" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R20" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D21" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F21" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G21" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H21" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="P21" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q21" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R21" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E22" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F22" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="H22" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="P22" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q22" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R22" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E23" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F23" t="s">
-        <v>163</v>
-      </c>
-      <c r="G23" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="H23" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="P23" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q23" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R23" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E24" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F24" t="s">
-        <v>164</v>
-      </c>
-      <c r="G24" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="H24" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="P24" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q24" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R24" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G25" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H25" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="P25" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q25" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R25" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E26" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F26" t="s">
-        <v>166</v>
-      </c>
-      <c r="G26" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="H26" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="P26" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q26" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R26" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D27" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E27" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F27" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G27" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H27" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="P27" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q27" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R27" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E28" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F28" t="s">
-        <v>168</v>
-      </c>
-      <c r="G28" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="H28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="P28" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q28" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R28" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" t="s">
         <v>143</v>
       </c>
-      <c r="E29" t="s">
-        <v>144</v>
-      </c>
       <c r="F29" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G29" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H29" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="P29" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q29" t="s">
+        <v>237</v>
+      </c>
+      <c r="R29" t="s">
+        <v>240</v>
+      </c>
+      <c r="S29" t="s">
         <v>243</v>
       </c>
-      <c r="R29" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18">
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E30" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F30" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G30" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H30" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="P30" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q30" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R30" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D31" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E31" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F31" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G31" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H31" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="P31" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q31" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R31" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
+        <v>240</v>
+      </c>
+      <c r="S31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
         <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D32" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G32" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H32" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="P32" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q32" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R32" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19">
+        <v>240</v>
+      </c>
+      <c r="S32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:46">
       <c r="A33" t="s">
         <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D33" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F33" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G33" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H33" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="P33" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q33" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R33" t="s">
+        <v>240</v>
+      </c>
+      <c r="S33" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:46">
       <c r="A34" t="s">
         <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D34" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E34" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F34" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G34" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="H34" t="s">
-        <v>224</v>
+        <v>210</v>
+      </c>
+      <c r="I34" t="s">
+        <v>220</v>
+      </c>
+      <c r="J34" t="s">
+        <v>225</v>
+      </c>
+      <c r="K34" t="s">
+        <v>229</v>
+      </c>
+      <c r="L34" t="s">
+        <v>230</v>
+      </c>
+      <c r="M34" t="s">
+        <v>231</v>
+      </c>
+      <c r="N34" t="s">
+        <v>232</v>
+      </c>
+      <c r="O34" t="s">
+        <v>225</v>
       </c>
       <c r="P34" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q34" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R34" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S34" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="35" spans="1:19">
+      <c r="T34" t="s">
+        <v>249</v>
+      </c>
+      <c r="U34" t="s">
+        <v>250</v>
+      </c>
+      <c r="V34" t="s">
+        <v>251</v>
+      </c>
+      <c r="W34" t="s">
+        <v>252</v>
+      </c>
+      <c r="X34" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN34" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO34" t="s">
+        <v>261</v>
+      </c>
+      <c r="AP34" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:46">
       <c r="A35" t="s">
         <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E35" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F35" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G35" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H35" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="P35" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q35" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R35" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19">
+        <v>240</v>
+      </c>
+      <c r="S35" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="36" spans="1:46">
       <c r="A36" t="s">
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D36" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E36" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F36" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G36" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H36" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="P36" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q36" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R36" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S36" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:46">
       <c r="A37" t="s">
         <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D37" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E37" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F37" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G37" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H37" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="P37" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q37" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R37" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:46">
       <c r="A38" t="s">
         <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F38" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G38" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H38" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="P38" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q38" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R38" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S38" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:46">
       <c r="A39" t="s">
         <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E39" t="s">
-        <v>144</v>
-      </c>
-      <c r="F39" t="s">
+        <v>138</v>
+      </c>
+      <c r="G39" t="s">
         <v>179</v>
       </c>
-      <c r="G39" t="s">
-        <v>190</v>
-      </c>
       <c r="H39" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="P39" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q39" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R39" t="s">
+        <v>240</v>
+      </c>
+      <c r="S39" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:46">
       <c r="A40" t="s">
         <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F40" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G40" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H40" t="s">
+        <v>216</v>
+      </c>
+      <c r="I40" t="s">
+        <v>176</v>
+      </c>
+      <c r="J40" t="s">
+        <v>226</v>
+      </c>
+      <c r="K40" t="s">
+        <v>229</v>
+      </c>
+      <c r="L40" t="s">
         <v>230</v>
       </c>
+      <c r="M40" t="s">
+        <v>231</v>
+      </c>
+      <c r="N40" t="s">
+        <v>232</v>
+      </c>
+      <c r="O40" t="s">
+        <v>226</v>
+      </c>
       <c r="P40" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q40" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R40" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S40" t="s">
+        <v>176</v>
+      </c>
+      <c r="T40" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="41" spans="1:19">
+      <c r="U40" t="s">
+        <v>250</v>
+      </c>
+      <c r="V40" t="s">
+        <v>251</v>
+      </c>
+      <c r="W40" t="s">
+        <v>252</v>
+      </c>
+      <c r="X40" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>255</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>256</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>256</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>257</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AO40" t="s">
+        <v>261</v>
+      </c>
+      <c r="AP40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:46">
       <c r="A41" t="s">
         <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D41" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E41" t="s">
-        <v>147</v>
-      </c>
-      <c r="F41" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="G41" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H41" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="P41" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q41" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R41" t="s">
-        <v>245</v>
-      </c>
-      <c r="S41" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="1:46">
       <c r="A42" t="s">
         <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E42" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F42" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G42" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H42" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="P42" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q42" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R42" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S42" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:46">
       <c r="A43" t="s">
         <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E43" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F43" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G43" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H43" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="P43" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q43" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R43" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S43" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:46">
       <c r="A44" t="s">
         <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E44" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F44" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="G44" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H44" t="s">
+        <v>210</v>
+      </c>
+      <c r="I44" t="s">
+        <v>221</v>
+      </c>
+      <c r="J44" t="s">
+        <v>227</v>
+      </c>
+      <c r="K44" t="s">
+        <v>229</v>
+      </c>
+      <c r="L44" t="s">
+        <v>230</v>
+      </c>
+      <c r="M44" t="s">
+        <v>231</v>
+      </c>
+      <c r="N44" t="s">
+        <v>232</v>
+      </c>
+      <c r="O44" t="s">
+        <v>227</v>
+      </c>
+      <c r="P44" t="s">
         <v>234</v>
       </c>
-      <c r="P44" t="s">
-        <v>241</v>
-      </c>
       <c r="Q44" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R44" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S44" t="s">
+        <v>242</v>
+      </c>
+      <c r="T44" t="s">
+        <v>249</v>
+      </c>
+      <c r="U44" t="s">
+        <v>250</v>
+      </c>
+      <c r="V44" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="W44" t="s">
+        <v>252</v>
+      </c>
+      <c r="X44" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>259</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL44" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AS44" t="s">
+        <v>263</v>
+      </c>
+      <c r="AT44" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="45" spans="1:46">
       <c r="A45" t="s">
         <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" t="s">
         <v>138</v>
       </c>
-      <c r="D45" t="s">
-        <v>143</v>
-      </c>
-      <c r="E45" t="s">
-        <v>147</v>
-      </c>
       <c r="F45" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G45" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H45" t="s">
-        <v>235</v>
+        <v>206</v>
+      </c>
+      <c r="I45" t="s">
+        <v>222</v>
+      </c>
+      <c r="J45" t="s">
+        <v>228</v>
+      </c>
+      <c r="K45" t="s">
+        <v>229</v>
+      </c>
+      <c r="L45" t="s">
+        <v>230</v>
+      </c>
+      <c r="M45" t="s">
+        <v>231</v>
+      </c>
+      <c r="N45" t="s">
+        <v>232</v>
+      </c>
+      <c r="O45" t="s">
+        <v>227</v>
       </c>
       <c r="P45" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q45" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R45" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="S45" t="s">
+        <v>242</v>
+      </c>
+      <c r="T45" t="s">
+        <v>249</v>
+      </c>
+      <c r="U45" t="s">
+        <v>250</v>
+      </c>
+      <c r="V45" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="46" spans="1:19">
+      <c r="W45" t="s">
+        <v>252</v>
+      </c>
+      <c r="X45" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>259</v>
+      </c>
+      <c r="AG45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP45" t="s">
+        <v>262</v>
+      </c>
+      <c r="AS45" t="s">
+        <v>263</v>
+      </c>
+      <c r="AT45" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="46" spans="1:46">
       <c r="A46" t="s">
         <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E46" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F46" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="G46" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H46" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="P46" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="Q46" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R46" t="s">
-        <v>245</v>
-      </c>
-      <c r="S46" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19">
-      <c r="A47" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" t="s">
-        <v>143</v>
-      </c>
-      <c r="E47" t="s">
-        <v>147</v>
-      </c>
-      <c r="F47" t="s">
-        <v>187</v>
-      </c>
-      <c r="G47" t="s">
-        <v>190</v>
-      </c>
-      <c r="H47" t="s">
-        <v>237</v>
-      </c>
-      <c r="P47" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>243</v>
-      </c>
-      <c r="R47" t="s">
-        <v>245</v>
-      </c>
-      <c r="S47" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19">
-      <c r="A48" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" t="s">
-        <v>141</v>
-      </c>
-      <c r="D48" t="s">
-        <v>143</v>
-      </c>
-      <c r="E48" t="s">
-        <v>147</v>
-      </c>
-      <c r="F48" t="s">
-        <v>188</v>
-      </c>
-      <c r="G48" t="s">
-        <v>190</v>
-      </c>
-      <c r="H48" t="s">
-        <v>238</v>
-      </c>
-      <c r="P48" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>243</v>
-      </c>
-      <c r="R48" t="s">
-        <v>245</v>
-      </c>
-      <c r="S48" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19">
-      <c r="A49" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" t="s">
-        <v>142</v>
-      </c>
-      <c r="D49" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" t="s">
-        <v>147</v>
-      </c>
-      <c r="F49" t="s">
-        <v>189</v>
-      </c>
-      <c r="G49" t="s">
-        <v>190</v>
-      </c>
-      <c r="H49" t="s">
-        <v>239</v>
-      </c>
-      <c r="P49" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>243</v>
-      </c>
-      <c r="R49" t="s">
-        <v>245</v>
-      </c>
-      <c r="S49" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>